<commit_message>
added object transformations in hits
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenten\Universiteit\Master EI\I-ComputerGraphics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Universiteit\MasterEI\I-ComputerGraphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D752B1-9E90-4F51-A026-0FE664F7BBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D871E2-0CF6-4B10-ABEC-87D866EE5979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26550" yWindow="0" windowWidth="22815" windowHeight="15600" xr2:uid="{7DF32E54-B2A1-4943-95EA-434693FB85FA}"/>
+    <workbookView xWindow="1608" yWindow="1092" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{7DF32E54-B2A1-4943-95EA-434693FB85FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sphere" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="52">
   <si>
     <t>Naam</t>
   </si>
@@ -93,12 +94,6 @@
     <t>Hit</t>
   </si>
   <si>
-    <t>target1</t>
-  </si>
-  <si>
-    <t>target2</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -178,6 +173,24 @@
   </si>
   <si>
     <t>ray20</t>
+  </si>
+  <si>
+    <t>hit1</t>
+  </si>
+  <si>
+    <t>hit2</t>
+  </si>
+  <si>
+    <t>3.3652256405</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>dir</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -187,7 +200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +213,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6897BB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -251,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -264,6 +283,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -580,18 +602,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB9E7C6-7885-4219-A16A-7CC110F17466}">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="14" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="C1" t="s">
         <v>2</v>
       </c>
@@ -599,17 +621,17 @@
         <v>17</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U1" s="3"/>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15" thickBot="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -638,27 +660,27 @@
         <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="Q2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="T2" s="4"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -684,14 +706,14 @@
         <v>15</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -714,10 +736,10 @@
         <v>7</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
@@ -730,11 +752,11 @@
       </c>
       <c r="Q4" s="3"/>
       <c r="T4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -757,10 +779,10 @@
         <v>7</v>
       </c>
       <c r="L5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N5" s="5">
         <v>0.77186560969999995</v>
@@ -783,7 +805,7 @@
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -806,25 +828,25 @@
         <v>7</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
-    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="15" thickBot="1">
       <c r="K7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N7" s="8">
         <v>-0.66062932809999997</v>
@@ -839,11 +861,11 @@
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -851,17 +873,17 @@
         <v>9</v>
       </c>
       <c r="L8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -890,10 +912,10 @@
         <v>9</v>
       </c>
       <c r="L9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N9" s="3">
         <v>-5</v>
@@ -906,11 +928,11 @@
       </c>
       <c r="Q9" s="3"/>
       <c r="T9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U9" s="3"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -939,10 +961,10 @@
         <v>9</v>
       </c>
       <c r="L10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N10" s="5">
         <v>-0.15061376839999999</v>
@@ -965,9 +987,9 @@
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -994,19 +1016,19 @@
         <v>9</v>
       </c>
       <c r="L11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
     </row>
-    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="15" thickBot="1">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -1033,10 +1055,10 @@
         <v>9</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N12" s="10">
         <v>-4.0548429193000004</v>
@@ -1051,13 +1073,13 @@
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
@@ -1084,19 +1106,19 @@
         <v>10</v>
       </c>
       <c r="L13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -1123,10 +1145,10 @@
         <v>10</v>
       </c>
       <c r="L14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N14" s="3">
         <v>2</v>
@@ -1139,13 +1161,13 @@
       </c>
       <c r="Q14" s="3"/>
       <c r="T14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U14" s="3"/>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" t="s">
         <v>31</v>
-      </c>
-      <c r="U14" s="3"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1172,10 +1194,10 @@
         <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N15" s="5">
         <v>1.5109583235999999</v>
@@ -1198,9 +1220,9 @@
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -1227,19 +1249,19 @@
         <v>10</v>
       </c>
       <c r="L16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
     </row>
-    <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="15" thickBot="1">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -1266,10 +1288,10 @@
         <v>10</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N17" s="10">
         <v>1.4810723697999999</v>
@@ -1284,13 +1306,13 @@
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="U17" s="3"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -1317,19 +1339,19 @@
         <v>11</v>
       </c>
       <c r="L18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
@@ -1356,10 +1378,10 @@
         <v>11</v>
       </c>
       <c r="L19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N19" s="3">
         <v>-2</v>
@@ -1372,13 +1394,13 @@
       </c>
       <c r="Q19" s="3"/>
       <c r="T19" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U19" s="3"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
@@ -1405,10 +1427,10 @@
         <v>11</v>
       </c>
       <c r="L20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N20" s="5">
         <v>-1.5520627463000001</v>
@@ -1431,9 +1453,9 @@
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>16</v>
@@ -1460,19 +1482,19 @@
         <v>11</v>
       </c>
       <c r="L21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
     </row>
-    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="15" thickBot="1">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
         <v>16</v>
@@ -1499,10 +1521,10 @@
         <v>11</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N22" s="10">
         <v>-1.2849028657999999</v>
@@ -1517,13 +1539,13 @@
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="U22" s="3"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
         <v>16</v>
@@ -1547,9 +1569,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
         <v>16</v>
@@ -1573,9 +1595,9 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
         <v>16</v>
@@ -1599,9 +1621,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
         <v>16</v>
@@ -1625,9 +1647,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
         <v>16</v>
@@ -1651,9 +1673,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
         <v>16</v>
@@ -1677,9 +1699,9 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
         <v>16</v>
@@ -1708,4 +1730,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A30BD3-27A3-4B36-9439-2FD6BC1D2A2B}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>-7</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5">
+        <v>-7</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>3.3652256404999998</v>
+      </c>
+      <c r="E6">
+        <v>2.4187246551000001</v>
+      </c>
+      <c r="F6">
+        <v>2.7973250492999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="D7">
+        <f>(D6-D5)/D4</f>
+        <v>0.79732504926923076</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:F7" si="0">(E6-E5)/E4</f>
+        <v>0.79732504927142855</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.79732504929999992</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
boolean objects added, not tested
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Universiteit\MasterEI\I-ComputerGraphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCED08B4-AF73-4F80-9755-F3338BF2EFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B41B86-BECD-4E98-BADF-C7354F1A6773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17700" yWindow="1335" windowWidth="17280" windowHeight="9075" xr2:uid="{7DF32E54-B2A1-4943-95EA-434693FB85FA}"/>
+    <workbookView xWindow="3576" yWindow="1968" windowWidth="17280" windowHeight="9072" xr2:uid="{7DF32E54-B2A1-4943-95EA-434693FB85FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sphere" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="52">
   <si>
     <t>Naam</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>hit2</t>
+  </si>
+  <si>
+    <t>-0.6165138327</t>
+  </si>
+  <si>
+    <t>0.155351777</t>
+  </si>
+  <si>
+    <t>0.0219192381</t>
+  </si>
+  <si>
+    <t>-0.6958923175</t>
   </si>
 </sst>
 </file>
@@ -580,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB9E7C6-7885-4219-A16A-7CC110F17466}">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:H17"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,20 +777,20 @@
       <c r="N5" s="5">
         <v>0.77186560969999995</v>
       </c>
-      <c r="O5" s="1">
-        <v>0.77186560969999995</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0.77186560969999995</v>
+      <c r="O5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="Q5" s="5">
         <v>0.77186560969999995</v>
       </c>
-      <c r="R5" s="1">
-        <v>0.77186560969999995</v>
-      </c>
-      <c r="S5" s="1">
-        <v>0.77186560969999995</v>
+      <c r="R5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>

</xml_diff>